<commit_message>
Updated basic skletion to all the tests
</commit_message>
<xml_diff>
--- a/AutomatedTest/TestData/Temenos/AutoDecisionProcess.xlsx
+++ b/AutomatedTest/TestData/Temenos/AutoDecisionProcess.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBD4AA6-FABD-488B-8B57-47C8BB353B00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A4176-8E1E-480D-8D05-428E1CD1C91F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,11 +12,12 @@
     <sheet name="InputTestData" sheetId="2" r:id="rId2"/>
     <sheet name="ValidationTestData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -8464,18 +8465,6 @@
     <t>AddStipulations</t>
   </si>
   <si>
-    <t>stipulation</t>
-  </si>
-  <si>
-    <t>requiredFor</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
     <t>2 years tax returns</t>
   </si>
   <si>
@@ -8494,18 +8483,9 @@
     <t>AccountNumber</t>
   </si>
   <si>
-    <t>Applicationtype</t>
-  </si>
-  <si>
     <t>ApproveApplyingFor</t>
   </si>
   <si>
-    <t>RejectApplyFor</t>
-  </si>
-  <si>
-    <t>ReviewApplyFor</t>
-  </si>
-  <si>
     <t>Auto: Automation Auto Approve</t>
   </si>
   <si>
@@ -8525,6 +8505,27 @@
   </si>
   <si>
     <t>Term</t>
+  </si>
+  <si>
+    <t>ApplicationType</t>
+  </si>
+  <si>
+    <t>RejectApplyingFor</t>
+  </si>
+  <si>
+    <t>ReviewApplyingFor</t>
+  </si>
+  <si>
+    <t>Stipulation0</t>
+  </si>
+  <si>
+    <t>RequiredFor0</t>
+  </si>
+  <si>
+    <t>Description0</t>
+  </si>
+  <si>
+    <t>Comments0</t>
   </si>
 </sst>
 </file>
@@ -21136,8 +21137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:CIU67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21162,46 +21163,46 @@
         <v>8</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>2826</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2818</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2827</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>2828</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>2816</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>2817</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>2822</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="I1" s="16" t="s">
         <v>2823</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="J1" s="16" t="s">
         <v>2824</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="K1" s="16" t="s">
         <v>2825</v>
       </c>
-      <c r="F1" s="17" t="s">
-        <v>2820</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>2821</v>
-      </c>
-      <c r="H1" s="17" t="s">
+      <c r="L1" s="16" t="s">
         <v>2829</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="M1" s="16" t="s">
         <v>2830</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>2831</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>2832</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>2812</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>2813</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>2814</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>2815</v>
       </c>
       <c r="P1" s="16" t="s">
         <v>13</v>
@@ -30406,13 +30407,13 @@
         <v>2803</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>2826</v>
+        <v>2819</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>2827</v>
+        <v>2820</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>2828</v>
+        <v>2821</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>2804</v>
@@ -30433,16 +30434,16 @@
         <v>2810</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>2816</v>
+        <v>2812</v>
       </c>
       <c r="M3" s="31" t="s">
-        <v>2817</v>
+        <v>2813</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>2818</v>
+        <v>2814</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>2819</v>
+        <v>2815</v>
       </c>
       <c r="P3" s="36" t="e">
         <f>#REF!</f>

</xml_diff>